<commit_message>
fix a bug relating to recentering roi
</commit_message>
<xml_diff>
--- a/dump_files/temp_data_xrv.xlsx
+++ b/dump_files/temp_data_xrv.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO4"/>
+  <dimension ref="A1:AO2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -665,7 +665,7 @@
         <v>0.1604804911245413</v>
       </c>
       <c r="J2" t="n">
-        <v>36.47288402410519</v>
+        <v>2.553180748865975</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -787,308 +787,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>13</v>
-      </c>
-      <c r="C3" t="n">
-        <v>23999</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.392421875</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.400292173376275</v>
-      </c>
-      <c r="G3" t="n">
-        <v>-0.01953125</v>
-      </c>
-      <c r="H3" t="n">
-        <v>14.62449438552168</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.1623516657921827</v>
-      </c>
-      <c r="J3" t="n">
-        <v>36.84504553115146</v>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>[[ 3.35175926e-09  1.28001579e-10  4.15417175e-10  5.58318835e-08
-  -1.34719743e-07  2.94366234e-07]
- [ 5.26209957e-12  8.88806639e-09 -5.87098428e-10 -6.72231035e-07
-  -3.72901214e-09  9.22736706e-09]
- [ 4.09373824e-11 -5.87098428e-10  4.63376893e-09  1.25435286e-06
-  -2.89774425e-08  3.96452922e-08]
- [ 9.89045436e-09 -6.72231035e-07  1.25435286e-06  3.90010225e-04
-  -7.00076293e-06  9.10870927e-06]
- [-2.51814660e-08 -3.72901214e-09 -2.89774425e-08 -7.00076293e-06
-   1.72730742e-05 -3.78453047e-05]
- [ 5.51818967e-08  9.22736706e-09  3.96452922e-08  9.10870927e-06
-  -3.78453047e-05  8.30719805e-05]]</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
-        <v>-0.2010163679237675</v>
-      </c>
-      <c r="M3" t="n">
-        <v>26.40176067418819</v>
-      </c>
-      <c r="N3" t="n">
-        <v>2.202868413645728</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.02379835718048294</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0.006886945032165119</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.3468727376230543</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0.01733133263297782</v>
-      </c>
-      <c r="S3" t="n">
-        <v>-0.007712573263520741</v>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>[[ 1.47588238e-08 -3.34991796e-09 -2.86757041e-09 -1.94658624e-07
-  -4.83347956e-07  6.64837188e-07]
- [-2.35046738e-10  6.11723244e-08  4.48093074e-08  4.03960244e-06
-   3.06636715e-08 -2.19347764e-07]
- [-2.36129767e-10  4.48093074e-08  5.69809328e-08  6.30338174e-06
-   3.08051347e-08 -2.59061552e-07]
- [-2.29813545e-08  4.03960244e-06  6.30338174e-06  7.42697023e-04
-   2.99810205e-06 -2.76652204e-05]
- [-7.87418636e-08  3.06636715e-08  3.08051347e-08  2.99810205e-06
-   9.13851492e-06 -1.25024966e-05]
- [ 1.07605980e-07 -2.19347764e-07 -2.59061552e-07 -2.76652204e-05
-  -1.25024966e-05  1.79486112e-05]]</t>
-        </is>
-      </c>
-      <c r="U3" t="n">
-        <v>-0.590791683442049</v>
-      </c>
-      <c r="V3" t="n">
-        <v>12.31944797701489</v>
-      </c>
-      <c r="W3" t="n">
-        <v>1.354265119328042</v>
-      </c>
-      <c r="X3" t="n">
-        <v>0.05100216599723046</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>0.01255269357825202</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>0.7116730859819469</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>-0.00827104435114088</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>0.02919019357618715</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>-0.5029745943664593</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>1.008999058819861</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>1.513504243010262</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>90.00002493749997</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>25.5029</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>6.775275000000001</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>11.09699999999999</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>49718</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AO3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>13</v>
-      </c>
-      <c r="C4" t="n">
-        <v>23999</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.387890625</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0.4110392172951939</v>
-      </c>
-      <c r="G4" t="n">
-        <v>-0.0196875</v>
-      </c>
-      <c r="H4" t="n">
-        <v>14.56170173348895</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.1619134804583391</v>
-      </c>
-      <c r="J4" t="n">
-        <v>36.69081052818206</v>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>[[ 3.51032102e-09  1.43850620e-10  4.72628467e-10  6.46940778e-08
-  -1.37853718e-07  3.00942025e-07]
- [ 5.11455338e-12  8.13095588e-09 -5.64205883e-10 -6.18028927e-07
-  -3.57378407e-09  8.92016113e-09]
- [ 4.11333504e-11 -5.64205883e-10  4.22034083e-09  1.15430810e-06
-  -2.87090429e-08  4.13131437e-08]
- [ 1.00545011e-08 -6.18028927e-07  1.15430810e-06  3.61122524e-04
-  -7.01736094e-06  9.67339440e-06]
- [-2.27828182e-08 -3.57378407e-09 -2.87090429e-08 -7.01736094e-06
-   1.54332824e-05 -3.37943453e-05]
- [ 4.98965054e-08  8.92016113e-09  4.13131437e-08  9.67339440e-06
-  -3.37943453e-05  7.41371991e-05]]</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
-        <v>-0.1991434820987736</v>
-      </c>
-      <c r="M4" t="n">
-        <v>26.28438158632956</v>
-      </c>
-      <c r="N4" t="n">
-        <v>2.202827074110476</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.02390463434166339</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0.006790984717259054</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0.3297938198398468</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.01876500467619497</v>
-      </c>
-      <c r="S4" t="n">
-        <v>-0.01077562721389261</v>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>[[ 1.50703138e-08 -3.57707002e-09 -3.02325755e-09 -2.04756072e-07
-  -4.90023195e-07  6.74368875e-07]
- [-7.79237288e-11  3.56761610e-08  2.59276469e-08  2.36959281e-06
-   1.00315821e-08 -1.16477559e-07]
- [-7.75214240e-11  2.59276469e-08  3.27242747e-08  3.66484272e-06
-   9.98005127e-09 -1.38282453e-07]
- [-7.63672493e-09  2.36959281e-06  3.66484272e-06  4.36826879e-04
-   9.83150926e-07 -1.50494823e-05]
- [-4.56639124e-08  1.00315821e-08  9.98005127e-09  9.83150926e-07
-   5.23342209e-06 -7.12963840e-06]
- [ 6.21695776e-08 -1.16477559e-07 -1.38282453e-07 -1.50494823e-05
-  -7.12963840e-06  1.01977769e-05]]</t>
-        </is>
-      </c>
-      <c r="U4" t="n">
-        <v>-0.5909360910168804</v>
-      </c>
-      <c r="V4" t="n">
-        <v>12.30151158501554</v>
-      </c>
-      <c r="W4" t="n">
-        <v>1.354267086614866</v>
-      </c>
-      <c r="X4" t="n">
-        <v>0.05107653042275818</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>0.01240245114469744</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>0.7047853649007698</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>-0.002483259171899697</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>0.02167290368083439</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>-0.5029748664092858</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>1.008996548441067</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>1.513503260684987</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>90.00002493749997</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>25.5029</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>6.775275000000001</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>11.09699999999999</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>49867</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AO4" t="b">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add possibility to show sym rods for selected rod in ubmate
</commit_message>
<xml_diff>
--- a/dump_files/temp_data_xrv.xlsx
+++ b/dump_files/temp_data_xrv.xlsx
@@ -644,138 +644,138 @@
         <v>13</v>
       </c>
       <c r="C2" t="n">
-        <v>23999</v>
+        <v>201</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.386484375</v>
+        <v>0.369375</v>
       </c>
       <c r="F2" t="n">
-        <v>0.3895451294573561</v>
+        <v>0.3569568925567829</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.019375</v>
+        <v>-0.029609375</v>
       </c>
       <c r="H2" t="n">
-        <v>14.38470768370964</v>
+        <v>15.65304865962676</v>
       </c>
       <c r="I2" t="n">
-        <v>0.1630193781351665</v>
+        <v>0.2394277101936094</v>
       </c>
       <c r="J2" t="n">
-        <v>25.20210797539058</v>
+        <v>77.64586441693002</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>[[ 3.34323263e-09  1.37253246e-10  4.48108361e-10  6.15178112e-08
-  -1.30800621e-07  2.85545815e-07]
- [ 5.02919562e-12  8.07071605e-09 -5.58822965e-10 -6.15817844e-07
-  -3.52227708e-09  8.81095146e-09]
- [ 4.07220739e-11 -5.58822965e-10  4.12996262e-09  1.13759582e-06
-  -2.84871382e-08  4.12720119e-08]
- [ 1.00247748e-08 -6.15817844e-07  1.13759582e-06  3.58721905e-04
-  -7.01264694e-06  9.74130915e-06]
- [-2.24539386e-08 -3.52227708e-09 -2.84871382e-08 -7.01264694e-06
-   1.52451431e-05 -3.33815694e-05]
- [ 4.91751047e-08  8.81095146e-09  4.12720119e-08  9.74130915e-06
-  -3.33815694e-05  7.32290460e-05]]</t>
+          <t>[[ 2.11883804e-09  2.18614701e-10  3.76726249e-10  2.91462550e-08
+  -1.73975983e-07  3.80124134e-07]
+ [ 4.66093519e-11  1.27223367e-08  2.50934392e-09  4.17531611e-07
+  -7.16715509e-09  7.91359046e-10]
+ [ 3.50531918e-11  2.50934392e-09  3.18934886e-09  1.18553331e-06
+  -5.38963933e-09 -4.80943059e-09]
+ [ 1.13743336e-08  4.17531611e-07  1.18553331e-06  4.77683950e-04
+  -1.74884994e-06 -2.18418660e-06]
+ [-2.64211871e-08 -7.16715509e-09 -5.38963933e-09 -1.74884994e-06
+   3.77024297e-06 -8.24896767e-06]
+ [ 5.78235104e-08  7.91359046e-10 -4.80943059e-09 -2.18418660e-06
+  -8.24896767e-06  1.81390155e-05]]</t>
         </is>
       </c>
       <c r="L2" t="n">
-        <v>-0.1995191749448844</v>
+        <v>0.09485455998490266</v>
       </c>
       <c r="M2" t="n">
-        <v>26.3703380250261</v>
+        <v>18.70175401583757</v>
       </c>
       <c r="N2" t="n">
-        <v>2.20283536651915</v>
+        <v>2.196356942856633</v>
       </c>
       <c r="O2" t="n">
-        <v>0.02382671508122759</v>
+        <v>0.0335967701310726</v>
       </c>
       <c r="P2" t="n">
-        <v>0.006749365298061104</v>
+        <v>0.004274572089244658</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.3310399441423864</v>
+        <v>0.5401422563457589</v>
       </c>
       <c r="R2" t="n">
-        <v>0.01955543805103895</v>
+        <v>-0.01231029476212248</v>
       </c>
       <c r="S2" t="n">
-        <v>-0.01269619445519747</v>
+        <v>0.05901414903216214</v>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>[[ 1.24920316e-08 -2.66258375e-09 -2.22615906e-09 -1.49386697e-07
-  -4.04619988e-07  5.55845343e-07]
- [-8.21472967e-11  4.71065846e-08  3.36866008e-08  3.19540080e-06
-   1.04204789e-08 -1.48795569e-07]
- [-8.18142685e-11  3.36866008e-08  4.35307493e-08  5.08036906e-06
-   1.03785922e-08 -1.80423383e-07]
- [-8.38119236e-09  3.19540080e-06  5.08036906e-06  6.29240770e-04
-   1.06320688e-06 -2.04914025e-05]
- [-6.44692578e-08  1.04204789e-08  1.03785922e-08  1.06320688e-06
-   7.33224650e-06 -9.97490996e-06]
- [ 8.76656103e-08 -1.48795569e-07 -1.80423383e-07 -2.04914025e-05
-  -9.97490996e-06  1.42190943e-05]]</t>
+          <t>[[ 1.33943563e-09 -2.97528621e-10 -3.20197919e-10 -2.86688100e-08
+  -9.79766332e-08  1.32895650e-07]
+ [-2.13374982e-11  2.45966841e-08  1.08710293e-08  2.68637174e-06
+   2.04567946e-09 -5.73241844e-08]
+ [-1.15006980e-11  1.08710293e-08  8.32423853e-09  2.37435420e-06
+   1.10268280e-09 -4.06791095e-08]
+ [-2.86713010e-09  2.68637174e-06  2.37435420e-06  7.01028091e-04
+   2.74902314e-07 -1.13392467e-05]
+ [-3.58898420e-08  2.04567946e-09  1.10268280e-09  2.74902314e-07
+   3.19052559e-06 -4.28320679e-06]
+ [ 4.81765169e-08 -5.73241844e-08 -4.06791095e-08 -1.13392467e-05
+  -4.28320679e-06  5.93899608e-06]]</t>
         </is>
       </c>
       <c r="U2" t="n">
-        <v>-0.5971245776998035</v>
+        <v>0.457217074810301</v>
       </c>
       <c r="V2" t="n">
-        <v>12.31190331064625</v>
+        <v>14.37017792968727</v>
       </c>
       <c r="W2" t="n">
-        <v>1.354351398701363</v>
+        <v>1.340136898903675</v>
       </c>
       <c r="X2" t="n">
-        <v>0.05103341984294531</v>
+        <v>0.04372378225184805</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.01199494571473045</v>
+        <v>0.004770433835121583</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.6582492635724109</v>
+        <v>0.3127109533062383</v>
       </c>
       <c r="AA2" t="n">
-        <v>-0.003382710706803671</v>
+        <v>-0.02000823415928051</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.02401624282889409</v>
+        <v>0.06172066823352594</v>
       </c>
       <c r="AC2" t="n">
-        <v>-0.5029742135069977</v>
+        <v>-1.00899797207166</v>
       </c>
       <c r="AD2" t="n">
-        <v>1.008995566122331</v>
+        <v>0.5044999538885565</v>
       </c>
       <c r="AE2" t="n">
-        <v>1.513508827211741</v>
+        <v>1.513497550107272</v>
       </c>
       <c r="AF2" t="n">
         <v>0</v>
       </c>
       <c r="AG2" t="n">
-        <v>90.00002493749997</v>
+        <v>0</v>
       </c>
       <c r="AH2" t="n">
-        <v>25.5029</v>
+        <v>-16.4081625</v>
       </c>
       <c r="AI2" t="n">
-        <v>6.775275000000001</v>
+        <v>6.704812499999999</v>
       </c>
       <c r="AJ2" t="n">
-        <v>11.09699999999999</v>
+        <v>11.139375</v>
       </c>
       <c r="AK2" t="n">
-        <v>0.7</v>
+        <v>0.34</v>
       </c>
       <c r="AL2" t="n">
-        <v>50177</v>
+        <v>85240</v>
       </c>
       <c r="AM2" t="n">
         <v>1</v>

</xml_diff>